<commit_message>
Add arquivo de manipulação e exportação
</commit_message>
<xml_diff>
--- a/Diagrama_logico-Excel.xlsx
+++ b/Diagrama_logico-Excel.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\44846245837\Desktop\SPMedGroup\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cliente\Desktop\Projeto_SPMedGroup\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{633E2E0B-A583-4E86-A85E-87C2261DB400}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -281,9 +282,6 @@
     <t>43522543-5</t>
   </si>
   <si>
-    <t>NULL</t>
-  </si>
-  <si>
     <t>Rua Estado de Israel 240, São Paulo, Estado de São Paulo, 04022-000</t>
   </si>
   <si>
@@ -303,12 +301,15 @@
   </si>
   <si>
     <t>Av. Paulista, 1578 - Bela Vista, São Paulo - SP, 01310-200</t>
+  </si>
+  <si>
+    <t>11 96584-5231</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -461,6 +462,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -473,17 +479,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -764,58 +765,58 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:S31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:G16"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
-    <col min="8" max="8" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="63.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="68.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="25.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="36.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B2" s="12" t="s">
+    <row r="2" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
       <c r="F2" s="7"/>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="10"/>
-      <c r="K2" s="8" t="s">
+      <c r="I2" s="13"/>
+      <c r="K2" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="10"/>
-      <c r="N2" s="8" t="s">
+      <c r="L2" s="13"/>
+      <c r="N2" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="9"/>
-      <c r="S2" s="10"/>
-    </row>
-    <row r="3" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12"/>
+      <c r="R2" s="12"/>
+      <c r="S2" s="13"/>
+    </row>
+    <row r="3" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
@@ -860,7 +861,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>1</v>
       </c>
@@ -905,7 +906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
@@ -942,7 +943,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
@@ -979,19 +980,19 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B8" s="11" t="s">
+    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B8" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-    </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>4</v>
       </c>
@@ -1010,12 +1011,12 @@
       <c r="G9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K9" s="14" t="s">
+      <c r="K9" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="14"/>
-    </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="L9" s="15"/>
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
         <v>1</v>
       </c>
@@ -1041,7 +1042,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
         <v>2</v>
       </c>
@@ -1067,7 +1068,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B12" s="2">
         <v>3</v>
       </c>
@@ -1093,7 +1094,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
         <v>4</v>
       </c>
@@ -1119,7 +1120,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B14" s="2">
         <v>5</v>
       </c>
@@ -1145,7 +1146,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B15" s="2">
         <v>6</v>
       </c>
@@ -1171,7 +1172,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B16" s="2">
         <v>7</v>
       </c>
@@ -1197,21 +1198,21 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
       <c r="K17" s="2">
         <v>7</v>
       </c>
       <c r="L17" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="N17" s="8" t="s">
+      <c r="N17" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="O17" s="9"/>
-      <c r="P17" s="9"/>
-      <c r="Q17" s="10"/>
-    </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="O17" s="12"/>
+      <c r="P17" s="12"/>
+      <c r="Q17" s="13"/>
+    </row>
+    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
       <c r="K18" s="2">
         <v>8</v>
       </c>
@@ -1231,7 +1232,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
       <c r="K19" s="2">
         <v>9</v>
       </c>
@@ -1241,7 +1242,7 @@
       <c r="N19" s="2">
         <v>1</v>
       </c>
-      <c r="O19" s="15" t="s">
+      <c r="O19" s="9" t="s">
         <v>52</v>
       </c>
       <c r="P19" s="2">
@@ -1251,17 +1252,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B20" s="11" t="s">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B20" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
       <c r="K20" s="2">
         <v>10</v>
       </c>
@@ -1271,7 +1272,7 @@
       <c r="N20" s="2">
         <v>2</v>
       </c>
-      <c r="O20" s="15" t="s">
+      <c r="O20" s="9" t="s">
         <v>55</v>
       </c>
       <c r="P20" s="2">
@@ -1281,7 +1282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
         <v>4</v>
       </c>
@@ -1315,7 +1316,7 @@
       <c r="N21" s="2">
         <v>3</v>
       </c>
-      <c r="O21" s="15" t="s">
+      <c r="O21" s="9" t="s">
         <v>58</v>
       </c>
       <c r="P21" s="2">
@@ -1325,7 +1326,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B22" s="2">
         <v>1</v>
       </c>
@@ -1336,7 +1337,7 @@
         <v>43164</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>78</v>
@@ -1348,7 +1349,7 @@
         <v>2</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K22" s="2">
         <v>12</v>
@@ -1357,7 +1358,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B23" s="2">
         <v>2</v>
       </c>
@@ -1380,7 +1381,7 @@
         <v>2</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K23" s="2">
         <v>13</v>
@@ -1389,7 +1390,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B24" s="2">
         <v>3</v>
       </c>
@@ -1412,7 +1413,7 @@
         <v>2</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K24" s="2">
         <v>14</v>
@@ -1421,7 +1422,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B25" s="2">
         <v>4</v>
       </c>
@@ -1444,7 +1445,7 @@
         <v>2</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K25" s="2">
         <v>15</v>
@@ -1453,7 +1454,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B26" s="2">
         <v>5</v>
       </c>
@@ -1476,7 +1477,7 @@
         <v>2</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K26" s="2">
         <v>16</v>
@@ -1485,7 +1486,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B27" s="2">
         <v>6</v>
       </c>
@@ -1508,7 +1509,7 @@
         <v>2</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K27" s="2">
         <v>17</v>
@@ -1517,7 +1518,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B28" s="2">
         <v>7</v>
       </c>
@@ -1540,21 +1541,21 @@
         <v>2</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
     </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
     </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
-      <c r="D31" s="16"/>
+      <c r="D31" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -1568,9 +1569,9 @@
     <mergeCell ref="B2:E2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="O19" r:id="rId1"/>
-    <hyperlink ref="O20" r:id="rId2"/>
-    <hyperlink ref="O21" r:id="rId3"/>
+    <hyperlink ref="O19" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="O20" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="O21" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>

</xml_diff>